<commit_message>
Datos cuestionarios, preguntas y respuestas
</commit_message>
<xml_diff>
--- a/recursos/DataBase/Base de Datos 035 v1.xlsx
+++ b/recursos/DataBase/Base de Datos 035 v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oavalos/Documents/Personal/Proyecto 035/Codigo/recursos/DataBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4D25FC-7625-9741-B18A-55CC36D8040D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A07D8D3-9D35-BB47-BE2F-926D859F4EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{D4FEB497-8318-AB43-A3DA-832786BD3E10}"/>
   </bookViews>
@@ -936,6 +936,72 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -963,24 +1029,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -988,54 +1036,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2129,8 +2129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B9ABE7-9E51-B84C-A716-4D1C8217E878}">
   <dimension ref="A1:AU77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ56" sqref="AJ56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2236,23 +2236,23 @@
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="Z6" s="130"/>
-      <c r="AA6" s="158" t="s">
+      <c r="AA6" s="140" t="s">
         <v>78</v>
       </c>
-      <c r="AB6" s="159"/>
-      <c r="AC6" s="159"/>
-      <c r="AD6" s="159"/>
-      <c r="AE6" s="160"/>
+      <c r="AB6" s="141"/>
+      <c r="AC6" s="141"/>
+      <c r="AD6" s="141"/>
+      <c r="AE6" s="142"/>
       <c r="AF6" s="131"/>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
-      <c r="AI6" s="146" t="s">
+      <c r="AI6" s="143" t="s">
         <v>81</v>
       </c>
-      <c r="AJ6" s="147"/>
-      <c r="AK6" s="147"/>
-      <c r="AL6" s="161"/>
-      <c r="AM6" s="148"/>
+      <c r="AJ6" s="144"/>
+      <c r="AK6" s="144"/>
+      <c r="AL6" s="145"/>
+      <c r="AM6" s="146"/>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
@@ -2448,22 +2448,22 @@
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
       <c r="AP11" s="1"/>
-      <c r="AQ11" s="143" t="s">
+      <c r="AQ11" s="147" t="s">
         <v>79</v>
       </c>
-      <c r="AR11" s="144"/>
-      <c r="AS11" s="144"/>
-      <c r="AT11" s="144"/>
-      <c r="AU11" s="145"/>
+      <c r="AR11" s="148"/>
+      <c r="AS11" s="148"/>
+      <c r="AT11" s="148"/>
+      <c r="AU11" s="149"/>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="S12" s="165" t="s">
+      <c r="S12" s="153" t="s">
         <v>85</v>
       </c>
-      <c r="T12" s="166"/>
-      <c r="U12" s="166"/>
-      <c r="V12" s="166"/>
-      <c r="W12" s="167"/>
+      <c r="T12" s="154"/>
+      <c r="U12" s="154"/>
+      <c r="V12" s="154"/>
+      <c r="W12" s="155"/>
       <c r="Z12" s="130"/>
       <c r="AA12" s="19"/>
       <c r="AB12" s="14" t="s">
@@ -2636,13 +2636,13 @@
       <c r="AF15" s="131"/>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
-      <c r="AI15" s="162" t="s">
+      <c r="AI15" s="150" t="s">
         <v>80</v>
       </c>
-      <c r="AJ15" s="163"/>
-      <c r="AK15" s="163"/>
-      <c r="AL15" s="163"/>
-      <c r="AM15" s="164"/>
+      <c r="AJ15" s="151"/>
+      <c r="AK15" s="151"/>
+      <c r="AL15" s="151"/>
+      <c r="AM15" s="152"/>
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
       <c r="AP15" s="1"/>
@@ -3003,13 +3003,13 @@
       </c>
       <c r="V25" s="75"/>
       <c r="W25" s="77"/>
-      <c r="AA25" s="152" t="s">
+      <c r="AA25" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="AB25" s="153"/>
-      <c r="AC25" s="153"/>
-      <c r="AD25" s="153"/>
-      <c r="AE25" s="154"/>
+      <c r="AB25" s="135"/>
+      <c r="AC25" s="135"/>
+      <c r="AD25" s="135"/>
+      <c r="AE25" s="136"/>
     </row>
     <row r="26" spans="11:47" x14ac:dyDescent="0.2">
       <c r="S26" s="76"/>
@@ -3132,13 +3132,13 @@
       <c r="W31" s="4"/>
     </row>
     <row r="32" spans="11:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K32" s="137" t="s">
+      <c r="K32" s="159" t="s">
         <v>87</v>
       </c>
-      <c r="L32" s="138"/>
-      <c r="M32" s="138"/>
-      <c r="N32" s="138"/>
-      <c r="O32" s="139"/>
+      <c r="L32" s="160"/>
+      <c r="M32" s="160"/>
+      <c r="N32" s="160"/>
+      <c r="O32" s="161"/>
       <c r="S32" s="88"/>
       <c r="T32" s="14" t="s">
         <v>7</v>
@@ -3176,13 +3176,13 @@
         <v>27</v>
       </c>
       <c r="W33" s="4"/>
-      <c r="AA33" s="143" t="s">
+      <c r="AA33" s="147" t="s">
         <v>112</v>
       </c>
-      <c r="AB33" s="144"/>
-      <c r="AC33" s="144"/>
-      <c r="AD33" s="144"/>
-      <c r="AE33" s="145"/>
+      <c r="AB33" s="148"/>
+      <c r="AC33" s="148"/>
+      <c r="AD33" s="148"/>
+      <c r="AE33" s="149"/>
     </row>
     <row r="34" spans="3:39" x14ac:dyDescent="0.2">
       <c r="K34" s="59" t="s">
@@ -3342,41 +3342,41 @@
     </row>
     <row r="45" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="3:39" x14ac:dyDescent="0.2">
-      <c r="C46" s="140" t="s">
+      <c r="C46" s="162" t="s">
         <v>86</v>
       </c>
-      <c r="D46" s="141"/>
-      <c r="E46" s="141"/>
-      <c r="F46" s="141"/>
-      <c r="G46" s="142"/>
-      <c r="K46" s="155" t="s">
+      <c r="D46" s="163"/>
+      <c r="E46" s="163"/>
+      <c r="F46" s="163"/>
+      <c r="G46" s="164"/>
+      <c r="K46" s="137" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="156"/>
-      <c r="M46" s="156"/>
-      <c r="N46" s="156"/>
-      <c r="O46" s="157"/>
-      <c r="S46" s="146" t="s">
+      <c r="L46" s="138"/>
+      <c r="M46" s="138"/>
+      <c r="N46" s="138"/>
+      <c r="O46" s="139"/>
+      <c r="S46" s="143" t="s">
         <v>84</v>
       </c>
-      <c r="T46" s="147"/>
-      <c r="U46" s="147"/>
-      <c r="V46" s="147"/>
-      <c r="W46" s="148"/>
-      <c r="AA46" s="149" t="s">
+      <c r="T46" s="144"/>
+      <c r="U46" s="144"/>
+      <c r="V46" s="144"/>
+      <c r="W46" s="146"/>
+      <c r="AA46" s="165" t="s">
         <v>83</v>
       </c>
-      <c r="AB46" s="150"/>
-      <c r="AC46" s="150"/>
-      <c r="AD46" s="150"/>
-      <c r="AE46" s="151"/>
-      <c r="AI46" s="152" t="s">
+      <c r="AB46" s="166"/>
+      <c r="AC46" s="166"/>
+      <c r="AD46" s="166"/>
+      <c r="AE46" s="167"/>
+      <c r="AI46" s="134" t="s">
         <v>82</v>
       </c>
-      <c r="AJ46" s="153"/>
-      <c r="AK46" s="153"/>
-      <c r="AL46" s="153"/>
-      <c r="AM46" s="154"/>
+      <c r="AJ46" s="135"/>
+      <c r="AK46" s="135"/>
+      <c r="AL46" s="135"/>
+      <c r="AM46" s="136"/>
     </row>
     <row r="47" spans="3:39" x14ac:dyDescent="0.2">
       <c r="C47" s="49" t="s">
@@ -4139,13 +4139,13 @@
     </row>
     <row r="64" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="11:24" x14ac:dyDescent="0.2">
-      <c r="S65" s="143" t="s">
+      <c r="S65" s="147" t="s">
         <v>109</v>
       </c>
-      <c r="T65" s="144"/>
-      <c r="U65" s="144"/>
-      <c r="V65" s="144"/>
-      <c r="W65" s="145"/>
+      <c r="T65" s="148"/>
+      <c r="U65" s="148"/>
+      <c r="V65" s="148"/>
+      <c r="W65" s="149"/>
     </row>
     <row r="66" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K66" s="86"/>
@@ -4216,13 +4216,13 @@
     </row>
     <row r="72" spans="11:24" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="11:24" x14ac:dyDescent="0.2">
-      <c r="S73" s="134" t="s">
+      <c r="S73" s="156" t="s">
         <v>110</v>
       </c>
-      <c r="T73" s="135"/>
-      <c r="U73" s="135"/>
-      <c r="V73" s="135"/>
-      <c r="W73" s="136"/>
+      <c r="T73" s="157"/>
+      <c r="U73" s="157"/>
+      <c r="V73" s="157"/>
+      <c r="W73" s="158"/>
     </row>
     <row r="74" spans="11:24" x14ac:dyDescent="0.2">
       <c r="S74" s="112" t="s">
@@ -4289,6 +4289,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="S73:W73"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="AA33:AE33"/>
+    <mergeCell ref="S46:W46"/>
+    <mergeCell ref="AA46:AE46"/>
+    <mergeCell ref="S65:W65"/>
     <mergeCell ref="AI46:AM46"/>
     <mergeCell ref="K46:O46"/>
     <mergeCell ref="AA6:AE6"/>
@@ -4297,13 +4304,6 @@
     <mergeCell ref="AI15:AM15"/>
     <mergeCell ref="S12:W12"/>
     <mergeCell ref="AA25:AE25"/>
-    <mergeCell ref="S73:W73"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="AA33:AE33"/>
-    <mergeCell ref="S46:W46"/>
-    <mergeCell ref="AA46:AE46"/>
-    <mergeCell ref="S65:W65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>